<commit_message>
update disposal plan: 소진계획_중국팀.xlsx
</commit_message>
<xml_diff>
--- a/data/disposal_uploads/소진계획_중국팀.xlsx
+++ b/data/disposal_uploads/소진계획_중국팀.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vd1p2\Downloads\소진계획_담당부서별_20260211 (1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54121AF-DC6D-4989-B364-BD5376974C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18039F3-2B2A-4FA2-8C04-DB64DF555D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="468">
   <si>
     <t>담당부서</t>
   </si>
@@ -1440,10 +1440,6 @@
   </si>
   <si>
     <t>12개월+</t>
-  </si>
-  <si>
-    <t>Test1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5644,7 +5640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -6127,7 +6125,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6181,7 +6179,7 @@
         <v>467</v>
       </c>
       <c r="H2" t="s">
-        <v>468</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -6207,7 +6205,7 @@
         <v>467</v>
       </c>
       <c r="H3" t="s">
-        <v>468</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -6233,7 +6231,7 @@
         <v>467</v>
       </c>
       <c r="H4" t="s">
-        <v>468</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -6259,7 +6257,7 @@
         <v>467</v>
       </c>
       <c r="H5" t="s">
-        <v>468</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -6285,7 +6283,7 @@
         <v>467</v>
       </c>
       <c r="H6" t="s">
-        <v>468</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -6311,7 +6309,7 @@
         <v>467</v>
       </c>
       <c r="H7" t="s">
-        <v>468</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>